<commit_message>
#162 fixed problem with code that adds extra permission records as part of the nightly service.
</commit_message>
<xml_diff>
--- a/BadgeList.xlsx
+++ b/BadgeList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="53">
   <si>
     <t>Image</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>Fifteen years of service</t>
+  </si>
+  <si>
+    <t>Completed Skills Inventory</t>
+  </si>
+  <si>
+    <t>Skills Assessment</t>
+  </si>
+  <si>
+    <t>I've got mad skillz</t>
+  </si>
+  <si>
+    <t>Completed the Magenic online skills inventory.</t>
+  </si>
+  <si>
+    <t>Completed PM Certification (such as PMP)</t>
+  </si>
+  <si>
+    <t>PM Certified</t>
   </si>
 </sst>
 </file>
@@ -1104,6 +1122,94 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="24444960"/>
+          <a:ext cx="1079365" cy="1269841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1079365</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1269841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="25725120"/>
+          <a:ext cx="1079365" cy="1269841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1079365</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1269841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="27020520"/>
           <a:ext cx="1079365" cy="1269841"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1381,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,15 +2023,58 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="E23" s="2"/>
+    <row r="22" spans="2:13" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="G23" s="2"/>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>

</xml_diff>